<commit_message>
changed files around, deleted some
</commit_message>
<xml_diff>
--- a/Fires.xlsx
+++ b/Fires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luis/Code/BigDataFinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4409D5F1-1674-9340-B636-D17B2A39D3D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60E2693-757C-B545-B306-1AC6284FB6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{D96FEB7F-44AB-FA47-9DDF-3B0615B72A44}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="208">
   <si>
     <t>Date</t>
   </si>
@@ -97,9 +97,6 @@
     <t>San Miguel</t>
   </si>
   <si>
-    <t>-</t>
-  </si>
-  <si>
     <t>INC-001</t>
   </si>
   <si>
@@ -544,18 +541,12 @@
     <t>San Pedro</t>
   </si>
   <si>
-    <t>No data</t>
-  </si>
-  <si>
     <t>Reserva Mbaracayu</t>
   </si>
   <si>
     <t>SSW</t>
   </si>
   <si>
-    <t>no data</t>
-  </si>
-  <si>
     <t>incendio de mas de 30 dias</t>
   </si>
   <si>
@@ -664,10 +655,10 @@
     <t>Wind Speed</t>
   </si>
   <si>
-    <t>Precipitacion</t>
-  </si>
-  <si>
     <t>Causes</t>
+  </si>
+  <si>
+    <t>Precipitation</t>
   </si>
 </sst>
 </file>
@@ -1030,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79AE7BB-29A4-0D4F-A0ED-DC6610B9D1DA}">
   <dimension ref="A1:AI101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="83" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="A102" sqref="A102:AN121"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1052,114 +1043,114 @@
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" t="s">
+        <v>206</v>
+      </c>
+      <c r="E1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F1" t="s">
+        <v>204</v>
+      </c>
+      <c r="G1" t="s">
+        <v>205</v>
+      </c>
+      <c r="H1" t="s">
+        <v>176</v>
+      </c>
+      <c r="I1" t="s">
         <v>177</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>178</v>
       </c>
-      <c r="D1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E1" t="s">
-        <v>209</v>
-      </c>
-      <c r="F1" t="s">
-        <v>207</v>
-      </c>
-      <c r="G1" t="s">
-        <v>208</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>179</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>180</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>181</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>182</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>183</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>184</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>185</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>186</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>187</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>188</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>189</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>190</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>191</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>192</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>193</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>194</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>195</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>196</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>197</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>198</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>199</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>200</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>201</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>202</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>203</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>204</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>205</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>44587</v>
@@ -1494,9 +1485,6 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
-        <v>20</v>
-      </c>
       <c r="G5">
         <v>0</v>
       </c>
@@ -1709,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="F7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G7">
         <v>45.06</v>
@@ -1923,7 +1911,7 @@
         <v>1.8</v>
       </c>
       <c r="F9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G9">
         <v>20.92</v>
@@ -2001,7 +1989,7 @@
         <v>-57.714300000000001</v>
       </c>
       <c r="AF9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AG9">
         <v>1</v>
@@ -2030,7 +2018,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G10">
         <v>9.65</v>
@@ -2108,7 +2096,7 @@
         <v>-57.6218</v>
       </c>
       <c r="AF10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AG10">
         <v>1</v>
@@ -2136,9 +2124,6 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
       <c r="G11">
         <v>0</v>
       </c>
@@ -2215,7 +2200,7 @@
         <v>-57.943899999999999</v>
       </c>
       <c r="AF11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG11">
         <v>1</v>
@@ -2229,7 +2214,7 @@
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="1">
         <v>44383</v>
@@ -2244,7 +2229,7 @@
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12">
         <v>8.0399999999999991</v>
@@ -2322,7 +2307,7 @@
         <v>-57.914200000000001</v>
       </c>
       <c r="AF12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="AG12">
         <v>1</v>
@@ -2336,7 +2321,7 @@
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="1">
         <v>44403</v>
@@ -2351,7 +2336,7 @@
         <v>12.1</v>
       </c>
       <c r="F13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13">
         <v>19.309999999999999</v>
@@ -2429,7 +2414,7 @@
         <v>-57.430599999999998</v>
       </c>
       <c r="AF13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AG13">
         <v>1</v>
@@ -2443,7 +2428,7 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B14" s="1">
         <v>44405</v>
@@ -2452,13 +2437,13 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14">
         <v>9.65</v>
@@ -2536,7 +2521,7 @@
         <v>-58.1541</v>
       </c>
       <c r="AF14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG14">
         <v>0</v>
@@ -2550,7 +2535,7 @@
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B15" s="1">
         <v>44417</v>
@@ -2643,7 +2628,7 @@
         <v>-57.241900000000001</v>
       </c>
       <c r="AF15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AG15">
         <v>1</v>
@@ -2657,7 +2642,7 @@
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="1">
         <v>44426</v>
@@ -2666,13 +2651,13 @@
         <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E16">
         <v>0</v>
       </c>
       <c r="F16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G16">
         <v>3.21</v>
@@ -2750,7 +2735,7 @@
         <v>-58.4664</v>
       </c>
       <c r="AF16" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AG16">
         <v>1</v>
@@ -2764,7 +2749,7 @@
     </row>
     <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>44427</v>
@@ -2779,7 +2764,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G17">
         <v>24.14</v>
@@ -2857,7 +2842,7 @@
         <v>-56.055399999999999</v>
       </c>
       <c r="AF17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG17">
         <v>1</v>
@@ -2871,7 +2856,7 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>44428</v>
@@ -2886,7 +2871,7 @@
         <v>0</v>
       </c>
       <c r="F18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G18">
         <v>28.96</v>
@@ -2964,7 +2949,7 @@
         <v>-56.055399999999999</v>
       </c>
       <c r="AF18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG18">
         <v>1</v>
@@ -2978,7 +2963,7 @@
     </row>
     <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>44428</v>
@@ -2993,7 +2978,7 @@
         <v>0</v>
       </c>
       <c r="F19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G19">
         <v>22.53</v>
@@ -3071,7 +3056,7 @@
         <v>-56.251300000000001</v>
       </c>
       <c r="AF19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="AG19">
         <v>1</v>
@@ -3085,7 +3070,7 @@
     </row>
     <row r="20" spans="1:35" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="3">
         <v>44428</v>
@@ -3094,13 +3079,10 @@
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E20">
         <v>0</v>
-      </c>
-      <c r="F20" t="s">
-        <v>20</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -3192,7 +3174,7 @@
     </row>
     <row r="21" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="1">
         <v>44429</v>
@@ -3285,7 +3267,7 @@
         <v>-56.055399999999999</v>
       </c>
       <c r="AF21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG21">
         <v>1</v>
@@ -3299,7 +3281,7 @@
     </row>
     <row r="22" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="1">
         <v>44429</v>
@@ -3392,7 +3374,7 @@
         <v>-56.012599999999999</v>
       </c>
       <c r="AF22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AG22">
         <v>0</v>
@@ -3406,7 +3388,7 @@
     </row>
     <row r="23" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B23" s="1">
         <v>44430</v>
@@ -3499,7 +3481,7 @@
         <v>-56.055399999999999</v>
       </c>
       <c r="AF23" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG23">
         <v>1</v>
@@ -3513,7 +3495,7 @@
     </row>
     <row r="24" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B24" s="1">
         <v>44430</v>
@@ -3528,7 +3510,7 @@
         <v>0</v>
       </c>
       <c r="F24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G24">
         <v>3.21</v>
@@ -3606,7 +3588,7 @@
         <v>-56.587800000000001</v>
       </c>
       <c r="AF24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG24">
         <v>0</v>
@@ -3620,7 +3602,7 @@
     </row>
     <row r="25" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B25" s="1">
         <v>44431</v>
@@ -3713,7 +3695,7 @@
         <v>-56.055399999999999</v>
       </c>
       <c r="AF25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG25">
         <v>1</v>
@@ -3727,7 +3709,7 @@
     </row>
     <row r="26" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B26" s="1">
         <v>44431</v>
@@ -3742,7 +3724,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G26">
         <v>4.82</v>
@@ -3820,7 +3802,7 @@
         <v>-56.587800000000001</v>
       </c>
       <c r="AF26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG26">
         <v>0</v>
@@ -3834,7 +3816,7 @@
     </row>
     <row r="27" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B27" s="1">
         <v>44431</v>
@@ -3843,13 +3825,13 @@
         <v>3</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27">
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G27">
         <v>20</v>
@@ -3927,7 +3909,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG27">
         <v>0</v>
@@ -3941,7 +3923,7 @@
     </row>
     <row r="28" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B28" s="1">
         <v>44432</v>
@@ -3956,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G28">
         <v>28.96</v>
@@ -4034,7 +4016,7 @@
         <v>-56.055399999999999</v>
       </c>
       <c r="AF28" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG28">
         <v>1</v>
@@ -4048,7 +4030,7 @@
     </row>
     <row r="29" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B29" s="1">
         <v>44432</v>
@@ -4063,7 +4045,7 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G29">
         <v>4.82</v>
@@ -4141,7 +4123,7 @@
         <v>-56.587800000000001</v>
       </c>
       <c r="AF29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AG29">
         <v>0</v>
@@ -4155,7 +4137,7 @@
     </row>
     <row r="30" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" s="1">
         <v>44432</v>
@@ -4164,13 +4146,13 @@
         <v>3</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E30">
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G30">
         <v>33</v>
@@ -4248,7 +4230,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG30">
         <v>0</v>
@@ -4262,7 +4244,7 @@
     </row>
     <row r="31" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B31" s="1">
         <v>44433</v>
@@ -4277,7 +4259,7 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G31">
         <v>33.79</v>
@@ -4355,7 +4337,7 @@
         <v>-56.055399999999999</v>
       </c>
       <c r="AF31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="AG31">
         <v>1</v>
@@ -4369,7 +4351,7 @@
     </row>
     <row r="32" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1">
         <v>44441</v>
@@ -4384,7 +4366,7 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G32">
         <v>20.92</v>
@@ -4462,7 +4444,7 @@
         <v>-57.5732</v>
       </c>
       <c r="AF32" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AG32">
         <v>1</v>
@@ -4476,7 +4458,7 @@
     </row>
     <row r="33" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1">
         <v>44453</v>
@@ -4490,9 +4472,6 @@
       <c r="E33">
         <v>0</v>
       </c>
-      <c r="F33" t="s">
-        <v>20</v>
-      </c>
       <c r="G33">
         <v>0</v>
       </c>
@@ -4569,7 +4548,7 @@
         <v>-55.690800000000003</v>
       </c>
       <c r="AF33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="AG33">
         <v>0</v>
@@ -4583,7 +4562,7 @@
     </row>
     <row r="34" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="1">
         <v>44476</v>
@@ -4592,13 +4571,13 @@
         <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E34">
         <v>0</v>
       </c>
       <c r="F34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G34">
         <v>3.21</v>
@@ -4676,7 +4655,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF34" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG34">
         <v>0</v>
@@ -4690,7 +4669,7 @@
     </row>
     <row r="35" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" s="1">
         <v>44495</v>
@@ -4699,13 +4678,13 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E35">
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G35">
         <v>8.0399999999999991</v>
@@ -4783,7 +4762,7 @@
         <v>-57.592199999999998</v>
       </c>
       <c r="AF35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="AG35">
         <v>0</v>
@@ -4797,7 +4776,7 @@
     </row>
     <row r="36" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B36" s="1">
         <v>44033</v>
@@ -4806,13 +4785,10 @@
         <v>10</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E36">
         <v>0</v>
-      </c>
-      <c r="F36" t="s">
-        <v>20</v>
       </c>
       <c r="G36">
         <v>0</v>
@@ -4890,7 +4866,7 @@
         <v>-60.044499999999999</v>
       </c>
       <c r="AF36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="AG36">
         <v>1</v>
@@ -4904,7 +4880,7 @@
     </row>
     <row r="37" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B37" s="1">
         <v>44034</v>
@@ -4913,13 +4889,13 @@
         <v>5.0000000000000001E-4</v>
       </c>
       <c r="D37" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E37">
         <v>0</v>
       </c>
       <c r="F37" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G37">
         <v>16.09</v>
@@ -4997,7 +4973,7 @@
         <v>-57.5565</v>
       </c>
       <c r="AF37" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AG37">
         <v>0</v>
@@ -5011,7 +4987,7 @@
     </row>
     <row r="38" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B38" s="1">
         <v>44041</v>
@@ -5020,13 +4996,13 @@
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E38">
         <v>0</v>
       </c>
       <c r="F38" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G38">
         <v>8</v>
@@ -5104,7 +5080,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG38">
         <v>0</v>
@@ -5118,7 +5094,7 @@
     </row>
     <row r="39" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B39" s="1">
         <v>44051</v>
@@ -5133,7 +5109,7 @@
         <v>0</v>
       </c>
       <c r="F39" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G39">
         <v>27.35</v>
@@ -5211,7 +5187,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG39">
         <v>0</v>
@@ -5225,7 +5201,7 @@
     </row>
     <row r="40" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="1">
         <v>44052</v>
@@ -5234,13 +5210,13 @@
         <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E40">
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G40">
         <v>19.309999999999999</v>
@@ -5318,7 +5294,7 @@
         <v>-57.478299999999997</v>
       </c>
       <c r="AF40" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="AG40">
         <v>0</v>
@@ -5332,7 +5308,7 @@
     </row>
     <row r="41" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B41" s="1">
         <v>44052</v>
@@ -5425,7 +5401,7 @@
         <v>-57.874499999999998</v>
       </c>
       <c r="AF41" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AG41">
         <v>1</v>
@@ -5439,7 +5415,7 @@
     </row>
     <row r="42" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B42" s="1">
         <v>44053</v>
@@ -5454,7 +5430,7 @@
         <v>0</v>
       </c>
       <c r="F42" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G42">
         <v>28.96</v>
@@ -5532,7 +5508,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF42" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG42">
         <v>0</v>
@@ -5546,7 +5522,7 @@
     </row>
     <row r="43" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" s="1">
         <v>44053</v>
@@ -5561,7 +5537,7 @@
         <v>0</v>
       </c>
       <c r="F43" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G43">
         <v>28.96</v>
@@ -5639,7 +5615,7 @@
         <v>-57.874499999999998</v>
       </c>
       <c r="AF43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AG43">
         <v>1</v>
@@ -5653,7 +5629,7 @@
     </row>
     <row r="44" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B44" s="1">
         <v>44053</v>
@@ -5662,13 +5638,13 @@
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E44">
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G44">
         <v>28.96</v>
@@ -5746,7 +5722,7 @@
         <v>-58.169600000000003</v>
       </c>
       <c r="AF44" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG44">
         <v>1</v>
@@ -5760,7 +5736,7 @@
     </row>
     <row r="45" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B45" s="1">
         <v>44060</v>
@@ -5775,7 +5751,7 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G45">
         <v>22.53</v>
@@ -5853,7 +5829,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF45" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG45">
         <v>0</v>
@@ -5867,7 +5843,7 @@
     </row>
     <row r="46" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B46" s="1">
         <v>44071</v>
@@ -5960,7 +5936,7 @@
         <v>-57.639299999999999</v>
       </c>
       <c r="AF46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="AG46">
         <v>0</v>
@@ -5974,7 +5950,7 @@
     </row>
     <row r="47" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B47" s="1">
         <v>44071</v>
@@ -6067,7 +6043,7 @@
         <v>-57.245399999999997</v>
       </c>
       <c r="AF47" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="AG47">
         <v>1</v>
@@ -6081,7 +6057,7 @@
     </row>
     <row r="48" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B48" s="1">
         <v>44073</v>
@@ -6090,13 +6066,13 @@
         <v>0.4</v>
       </c>
       <c r="D48" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E48">
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G48">
         <v>25.74</v>
@@ -6174,7 +6150,7 @@
         <v>-57.641199999999998</v>
       </c>
       <c r="AF48" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AG48">
         <v>0</v>
@@ -6188,7 +6164,7 @@
     </row>
     <row r="49" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B49" s="1">
         <v>44074</v>
@@ -6197,13 +6173,13 @@
         <v>0.5</v>
       </c>
       <c r="D49" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E49">
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G49">
         <v>22.53</v>
@@ -6281,7 +6257,7 @@
         <v>-57.641199999999998</v>
       </c>
       <c r="AF49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="AG49">
         <v>0</v>
@@ -6295,7 +6271,7 @@
     </row>
     <row r="50" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B50" s="1">
         <v>44078</v>
@@ -6310,7 +6286,7 @@
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G50">
         <v>19.309999999999999</v>
@@ -6388,7 +6364,7 @@
         <v>-55.937100000000001</v>
       </c>
       <c r="AF50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="AG50">
         <v>0</v>
@@ -6402,7 +6378,7 @@
     </row>
     <row r="51" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B51" s="1">
         <v>44086</v>
@@ -6416,9 +6392,6 @@
       <c r="E51">
         <v>0</v>
       </c>
-      <c r="F51" t="s">
-        <v>20</v>
-      </c>
       <c r="G51">
         <v>0</v>
       </c>
@@ -6495,7 +6468,7 @@
         <v>-57.127200000000002</v>
       </c>
       <c r="AF51" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="AG51">
         <v>0</v>
@@ -6509,7 +6482,7 @@
     </row>
     <row r="52" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B52" s="1">
         <v>44088</v>
@@ -6518,13 +6491,13 @@
         <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E52">
         <v>1.9</v>
       </c>
       <c r="F52" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G52">
         <v>25.74</v>
@@ -6602,7 +6575,7 @@
         <v>-57.348399999999998</v>
       </c>
       <c r="AF52" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="AG52">
         <v>0</v>
@@ -6616,7 +6589,7 @@
     </row>
     <row r="53" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="1">
         <v>44093</v>
@@ -6630,9 +6603,6 @@
       <c r="E53">
         <v>0</v>
       </c>
-      <c r="F53" t="s">
-        <v>20</v>
-      </c>
       <c r="G53">
         <v>0</v>
       </c>
@@ -6703,13 +6673,13 @@
         <v>33</v>
       </c>
       <c r="AD53">
-        <v>-25.637080000000001</v>
+        <v>-25.6371</v>
       </c>
       <c r="AE53">
-        <v>-54.595089999999999</v>
+        <v>-54.595100000000002</v>
       </c>
       <c r="AF53" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="AG53">
         <v>0</v>
@@ -6723,7 +6693,7 @@
     </row>
     <row r="54" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B54" s="1">
         <v>44094</v>
@@ -6738,7 +6708,7 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G54">
         <v>14.48</v>
@@ -6816,7 +6786,7 @@
         <v>-55.746200000000002</v>
       </c>
       <c r="AF54" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AG54">
         <v>0</v>
@@ -6830,7 +6800,7 @@
     </row>
     <row r="55" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B55" s="1">
         <v>44095</v>
@@ -6839,13 +6809,13 @@
         <v>2</v>
       </c>
       <c r="D55" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E55">
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G55">
         <v>11.26</v>
@@ -6923,7 +6893,7 @@
         <v>-55.746200000000002</v>
       </c>
       <c r="AF55" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AG55">
         <v>0</v>
@@ -6937,7 +6907,7 @@
     </row>
     <row r="56" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B56" s="1">
         <v>44096</v>
@@ -6946,7 +6916,7 @@
         <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -7030,7 +7000,7 @@
         <v>-55.746200000000002</v>
       </c>
       <c r="AF56" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AG56">
         <v>0</v>
@@ -7044,7 +7014,7 @@
     </row>
     <row r="57" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B57" s="1">
         <v>44097</v>
@@ -7053,13 +7023,13 @@
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E57">
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G57">
         <v>9.65</v>
@@ -7137,7 +7107,7 @@
         <v>-55.746200000000002</v>
       </c>
       <c r="AF57" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AG57">
         <v>0</v>
@@ -7151,7 +7121,7 @@
     </row>
     <row r="58" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B58" s="1">
         <v>44098</v>
@@ -7160,13 +7130,10 @@
         <v>0</v>
       </c>
       <c r="D58" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E58">
         <v>0</v>
-      </c>
-      <c r="F58" t="s">
-        <v>20</v>
       </c>
       <c r="G58">
         <v>0</v>
@@ -7244,7 +7211,7 @@
         <v>-55.746200000000002</v>
       </c>
       <c r="AF58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AG58">
         <v>0</v>
@@ -7258,7 +7225,7 @@
     </row>
     <row r="59" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B59" s="1">
         <v>44100</v>
@@ -7267,7 +7234,7 @@
         <v>2.4</v>
       </c>
       <c r="D59" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -7351,7 +7318,7 @@
         <v>-54.579700000000003</v>
       </c>
       <c r="AF59" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="AG59">
         <v>0</v>
@@ -7365,7 +7332,7 @@
     </row>
     <row r="60" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B60" s="1">
         <v>44100</v>
@@ -7374,13 +7341,13 @@
         <v>1.2</v>
       </c>
       <c r="D60" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E60">
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G60">
         <v>3.7</v>
@@ -7458,7 +7425,7 @@
         <v>-54.457700000000003</v>
       </c>
       <c r="AF60" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="AG60">
         <v>0</v>
@@ -7472,7 +7439,7 @@
     </row>
     <row r="61" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B61" s="1">
         <v>44116</v>
@@ -7481,7 +7448,7 @@
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E61">
         <v>1.1000000000000001</v>
@@ -7498,9 +7465,6 @@
       <c r="I61">
         <v>30</v>
       </c>
-      <c r="J61" t="s">
-        <v>20</v>
-      </c>
       <c r="K61">
         <v>25</v>
       </c>
@@ -7531,9 +7495,6 @@
       <c r="T61">
         <v>41</v>
       </c>
-      <c r="U61" t="s">
-        <v>20</v>
-      </c>
       <c r="V61">
         <v>35</v>
       </c>
@@ -7565,7 +7526,7 @@
         <v>-58.167900000000003</v>
       </c>
       <c r="AF61" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG61">
         <v>1</v>
@@ -7579,7 +7540,7 @@
     </row>
     <row r="62" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B62" s="1">
         <v>44117</v>
@@ -7588,7 +7549,7 @@
         <v>2</v>
       </c>
       <c r="D62" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E62">
         <v>6.6</v>
@@ -7602,9 +7563,6 @@
       <c r="H62">
         <v>30</v>
       </c>
-      <c r="I62" t="s">
-        <v>20</v>
-      </c>
       <c r="J62">
         <v>25</v>
       </c>
@@ -7635,9 +7593,6 @@
       <c r="S62">
         <v>41</v>
       </c>
-      <c r="T62" t="s">
-        <v>20</v>
-      </c>
       <c r="U62">
         <v>35</v>
       </c>
@@ -7672,7 +7627,7 @@
         <v>-58.167900000000003</v>
       </c>
       <c r="AF62" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG62">
         <v>1</v>
@@ -7686,7 +7641,7 @@
     </row>
     <row r="63" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B63" s="1">
         <v>44118</v>
@@ -7695,20 +7650,17 @@
         <v>2</v>
       </c>
       <c r="D63" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E63">
         <v>7.7</v>
       </c>
       <c r="F63" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G63">
         <v>7</v>
       </c>
-      <c r="H63" t="s">
-        <v>20</v>
-      </c>
       <c r="I63">
         <v>25</v>
       </c>
@@ -7739,9 +7691,6 @@
       <c r="R63">
         <v>24</v>
       </c>
-      <c r="S63" t="s">
-        <v>20</v>
-      </c>
       <c r="T63">
         <v>35</v>
       </c>
@@ -7779,7 +7728,7 @@
         <v>-58.167900000000003</v>
       </c>
       <c r="AF63" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG63">
         <v>1</v>
@@ -7793,7 +7742,7 @@
     </row>
     <row r="64" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B64" s="1">
         <v>44118</v>
@@ -7802,13 +7751,13 @@
         <v>2</v>
       </c>
       <c r="D64" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E64">
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G64">
         <v>19.11</v>
@@ -7886,7 +7835,7 @@
         <v>-58.167900000000003</v>
       </c>
       <c r="AF64" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="AG64">
         <v>1</v>
@@ -7900,7 +7849,7 @@
     </row>
     <row r="65" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B65" s="1">
         <v>44119</v>
@@ -7909,20 +7858,17 @@
         <v>2</v>
       </c>
       <c r="D65" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E65">
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G65">
         <v>25.35</v>
       </c>
-      <c r="H65" t="s">
-        <v>20</v>
-      </c>
       <c r="I65">
         <v>20</v>
       </c>
@@ -7953,9 +7899,6 @@
       <c r="R65">
         <v>25</v>
       </c>
-      <c r="S65" t="s">
-        <v>20</v>
-      </c>
       <c r="T65">
         <v>31</v>
       </c>
@@ -7993,7 +7936,7 @@
         <v>-55.782899999999998</v>
       </c>
       <c r="AF65" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AG65">
         <v>0</v>
@@ -8007,7 +7950,7 @@
     </row>
     <row r="66" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B66" s="1">
         <v>44138</v>
@@ -8016,13 +7959,13 @@
         <v>150</v>
       </c>
       <c r="D66" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E66">
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G66">
         <v>10.99</v>
@@ -8100,7 +8043,7 @@
         <v>-57.642400000000002</v>
       </c>
       <c r="AF66" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="AG66">
         <v>1</v>
@@ -8114,7 +8057,7 @@
     </row>
     <row r="67" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B67" s="1">
         <v>44140</v>
@@ -8207,7 +8150,7 @@
         <v>-57.159100000000002</v>
       </c>
       <c r="AF67" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AG67">
         <v>0</v>
@@ -8221,7 +8164,7 @@
     </row>
     <row r="68" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B68" s="1">
         <v>43693</v>
@@ -8230,13 +8173,13 @@
         <v>0</v>
       </c>
       <c r="D68" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E68">
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G68">
         <v>10.99</v>
@@ -8314,7 +8257,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG68">
         <v>0</v>
@@ -8328,7 +8271,7 @@
     </row>
     <row r="69" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B69" s="1">
         <v>43694</v>
@@ -8337,13 +8280,13 @@
         <v>0</v>
       </c>
       <c r="D69" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E69">
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G69">
         <v>28</v>
@@ -8421,7 +8364,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF69" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG69">
         <v>0</v>
@@ -8435,7 +8378,7 @@
     </row>
     <row r="70" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B70" s="1">
         <v>43695</v>
@@ -8444,13 +8387,13 @@
         <v>0</v>
       </c>
       <c r="D70" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E70">
         <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G70">
         <v>16.989999999999998</v>
@@ -8528,7 +8471,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG70">
         <v>0</v>
@@ -8542,7 +8485,7 @@
     </row>
     <row r="71" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B71" s="1">
         <v>43696</v>
@@ -8551,7 +8494,7 @@
         <v>0</v>
       </c>
       <c r="D71" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -8635,7 +8578,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF71" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG71">
         <v>0</v>
@@ -8649,7 +8592,7 @@
     </row>
     <row r="72" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B72" s="1">
         <v>43697</v>
@@ -8658,7 +8601,7 @@
         <v>220</v>
       </c>
       <c r="D72" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -8742,7 +8685,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF72" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG72">
         <v>0</v>
@@ -8756,7 +8699,7 @@
     </row>
     <row r="73" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B73" s="1">
         <v>44063</v>
@@ -8765,13 +8708,13 @@
         <v>100</v>
       </c>
       <c r="D73" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E73">
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G73">
         <v>12.98</v>
@@ -8849,7 +8792,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF73" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG73">
         <v>0</v>
@@ -8863,7 +8806,7 @@
     </row>
     <row r="74" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B74" s="1">
         <v>43699</v>
@@ -8872,13 +8815,13 @@
         <v>0</v>
       </c>
       <c r="D74" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E74">
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G74">
         <v>7</v>
@@ -8956,7 +8899,7 @@
         <v>-58.1693</v>
       </c>
       <c r="AF74" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG74">
         <v>0</v>
@@ -8970,7 +8913,7 @@
     </row>
     <row r="75" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B75" s="1">
         <v>43700</v>
@@ -8979,13 +8922,13 @@
         <v>0</v>
       </c>
       <c r="D75" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E75">
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G75">
         <v>7</v>
@@ -9063,7 +9006,7 @@
         <v>-58.1693</v>
       </c>
       <c r="AF75" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG75">
         <v>0</v>
@@ -9077,7 +9020,7 @@
     </row>
     <row r="76" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B76" s="1">
         <v>43701</v>
@@ -9086,13 +9029,13 @@
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E76">
         <v>0</v>
       </c>
       <c r="F76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G76">
         <v>7</v>
@@ -9170,7 +9113,7 @@
         <v>-58.1693</v>
       </c>
       <c r="AF76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG76">
         <v>0</v>
@@ -9184,7 +9127,7 @@
     </row>
     <row r="77" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B77" s="1">
         <v>43701</v>
@@ -9193,13 +9136,13 @@
         <v>2</v>
       </c>
       <c r="D77" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E77">
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G77">
         <v>7</v>
@@ -9277,7 +9220,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF77" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG77">
         <v>0</v>
@@ -9291,7 +9234,7 @@
     </row>
     <row r="78" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B78" s="1">
         <v>43702</v>
@@ -9300,7 +9243,7 @@
         <v>190</v>
       </c>
       <c r="D78" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E78">
         <v>0</v>
@@ -9384,7 +9327,7 @@
         <v>-58.1693</v>
       </c>
       <c r="AF78" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG78">
         <v>0</v>
@@ -9398,7 +9341,7 @@
     </row>
     <row r="79" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B79" s="1">
         <v>43702</v>
@@ -9407,7 +9350,7 @@
         <v>2</v>
       </c>
       <c r="D79" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E79">
         <v>0</v>
@@ -9491,7 +9434,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF79" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG79">
         <v>0</v>
@@ -9505,7 +9448,7 @@
     </row>
     <row r="80" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B80" s="1">
         <v>43703</v>
@@ -9514,7 +9457,7 @@
         <v>2</v>
       </c>
       <c r="D80" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -9598,7 +9541,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF80" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG80">
         <v>0</v>
@@ -9612,7 +9555,7 @@
     </row>
     <row r="81" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B81" s="1">
         <v>43707</v>
@@ -9621,13 +9564,13 @@
         <v>212.42</v>
       </c>
       <c r="D81" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E81">
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G81">
         <v>16.989999999999998</v>
@@ -9705,7 +9648,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF81" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG81">
         <v>0</v>
@@ -9719,7 +9662,7 @@
     </row>
     <row r="82" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B82" s="1">
         <v>43707</v>
@@ -9728,13 +9671,13 @@
         <v>473.33</v>
       </c>
       <c r="D82" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E82">
         <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G82">
         <v>16.989999999999998</v>
@@ -9812,7 +9755,7 @@
         <v>-58.1693</v>
       </c>
       <c r="AF82" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="AG82">
         <v>0</v>
@@ -9826,16 +9769,13 @@
     </row>
     <row r="83" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B83" s="1">
         <v>43709</v>
       </c>
-      <c r="C83" t="s">
-        <v>169</v>
-      </c>
       <c r="D83" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E83">
         <v>0</v>
@@ -9919,7 +9859,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF83" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG83">
         <v>0</v>
@@ -9933,16 +9873,13 @@
     </row>
     <row r="84" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B84" s="1">
         <v>43713</v>
       </c>
-      <c r="C84" t="s">
-        <v>169</v>
-      </c>
       <c r="D84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E84">
         <v>0</v>
@@ -10026,7 +9963,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG84">
         <v>0</v>
@@ -10040,22 +9977,19 @@
     </row>
     <row r="85" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B85" s="1">
         <v>43714</v>
       </c>
-      <c r="C85" t="s">
-        <v>169</v>
-      </c>
       <c r="D85" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E85">
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G85">
         <v>7</v>
@@ -10133,7 +10067,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF85" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG85">
         <v>0</v>
@@ -10147,22 +10081,19 @@
     </row>
     <row r="86" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B86" s="1">
         <v>43715</v>
       </c>
-      <c r="C86" t="s">
-        <v>169</v>
-      </c>
       <c r="D86" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E86">
         <v>0</v>
       </c>
       <c r="F86" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G86">
         <v>21.88</v>
@@ -10240,7 +10171,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF86" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG86">
         <v>0</v>
@@ -10254,22 +10185,19 @@
     </row>
     <row r="87" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B87" s="1">
         <v>43716</v>
       </c>
-      <c r="C87" t="s">
-        <v>169</v>
-      </c>
       <c r="D87" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E87">
         <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G87">
         <v>26</v>
@@ -10347,7 +10275,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF87" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG87">
         <v>0</v>
@@ -10361,22 +10289,19 @@
     </row>
     <row r="88" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B88" s="1">
         <v>43717</v>
       </c>
-      <c r="C88" t="s">
-        <v>169</v>
-      </c>
       <c r="D88" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E88">
         <v>0</v>
       </c>
       <c r="F88" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G88">
         <v>26</v>
@@ -10454,7 +10379,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG88">
         <v>0</v>
@@ -10468,7 +10393,7 @@
     </row>
     <row r="89" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B89" s="1">
         <v>43717</v>
@@ -10483,7 +10408,7 @@
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G89">
         <v>26</v>
@@ -10561,7 +10486,7 @@
         <v>-55.441800000000001</v>
       </c>
       <c r="AF89" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="AG89">
         <v>0</v>
@@ -10575,7 +10500,7 @@
     </row>
     <row r="90" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B90" s="1">
         <v>43717</v>
@@ -10590,7 +10515,7 @@
         <v>0</v>
       </c>
       <c r="F90" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G90">
         <v>19.98</v>
@@ -10668,7 +10593,7 @@
         <v>-56.182400000000001</v>
       </c>
       <c r="AF90" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AG90">
         <v>1</v>
@@ -10682,7 +10607,7 @@
     </row>
     <row r="91" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B91" s="1">
         <v>43718</v>
@@ -10697,7 +10622,7 @@
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G91">
         <v>17.989999999999998</v>
@@ -10775,7 +10700,7 @@
         <v>-56.182400000000001</v>
       </c>
       <c r="AF91" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="AG91">
         <v>1</v>
@@ -10789,7 +10714,7 @@
     </row>
     <row r="92" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B92" s="1">
         <v>43725</v>
@@ -10798,7 +10723,7 @@
         <v>2412.9899999999998</v>
       </c>
       <c r="D92" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E92">
         <v>0</v>
@@ -10882,7 +10807,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF92" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG92">
         <v>0</v>
@@ -10896,16 +10821,13 @@
     </row>
     <row r="93" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B93" s="1">
         <v>43726</v>
       </c>
-      <c r="C93" t="s">
-        <v>172</v>
-      </c>
       <c r="D93" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E93">
         <v>0</v>
@@ -10989,7 +10911,7 @@
         <v>-58.165900000000001</v>
       </c>
       <c r="AF93" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG93">
         <v>0</v>
@@ -11003,22 +10925,19 @@
     </row>
     <row r="94" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B94" s="1">
         <v>43727</v>
       </c>
-      <c r="C94" t="s">
-        <v>172</v>
-      </c>
       <c r="D94" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E94">
         <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G94">
         <v>23.99</v>
@@ -11096,7 +11015,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF94" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG94">
         <v>0</v>
@@ -11110,16 +11029,13 @@
     </row>
     <row r="95" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B95" s="1">
         <v>43728</v>
       </c>
-      <c r="C95" t="s">
-        <v>172</v>
-      </c>
       <c r="D95" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E95">
         <v>0.3</v>
@@ -11203,7 +11119,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF95" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG95">
         <v>0</v>
@@ -11217,22 +11133,19 @@
     </row>
     <row r="96" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B96" s="1">
         <v>43729</v>
       </c>
-      <c r="C96" t="s">
-        <v>169</v>
-      </c>
       <c r="D96" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E96">
         <v>0</v>
       </c>
       <c r="F96" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G96">
         <v>8.99</v>
@@ -11310,7 +11223,7 @@
         <v>-59.121699999999997</v>
       </c>
       <c r="AF96" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="AG96">
         <v>0</v>
@@ -11324,7 +11237,7 @@
     </row>
     <row r="97" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B97" s="1">
         <v>43729</v>
@@ -11339,7 +11252,7 @@
         <v>0</v>
       </c>
       <c r="F97" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="G97">
         <v>4.9800000000000004</v>
@@ -11417,7 +11330,7 @@
         <v>-57.874499999999998</v>
       </c>
       <c r="AF97" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="AG97">
         <v>1</v>
@@ -11431,7 +11344,7 @@
     </row>
     <row r="98" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B98" s="1">
         <v>43732</v>
@@ -11440,7 +11353,7 @@
         <v>3.5</v>
       </c>
       <c r="D98" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E98">
         <v>0</v>
@@ -11524,7 +11437,7 @@
         <v>-55.782899999999998</v>
       </c>
       <c r="AF98" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AG98">
         <v>0</v>
@@ -11538,7 +11451,7 @@
     </row>
     <row r="99" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B99" s="1">
         <v>43738</v>
@@ -11547,13 +11460,13 @@
         <v>0</v>
       </c>
       <c r="D99" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E99">
         <v>0</v>
       </c>
       <c r="F99" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G99">
         <v>25.99</v>
@@ -11631,7 +11544,7 @@
         <v>-55.746200000000002</v>
       </c>
       <c r="AF99" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AG99">
         <v>0</v>
@@ -11645,7 +11558,7 @@
     </row>
     <row r="100" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B100" s="1">
         <v>43739</v>
@@ -11654,13 +11567,13 @@
         <v>0</v>
       </c>
       <c r="D100" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E100">
         <v>0</v>
       </c>
       <c r="F100" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G100">
         <v>25.99</v>
@@ -11738,7 +11651,7 @@
         <v>-55.746200000000002</v>
       </c>
       <c r="AF100" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AG100">
         <v>0</v>
@@ -11752,7 +11665,7 @@
     </row>
     <row r="101" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B101" s="1">
         <v>43740</v>
@@ -11761,13 +11674,13 @@
         <v>0.5</v>
       </c>
       <c r="D101" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E101">
         <v>3.4</v>
       </c>
       <c r="F101" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="G101">
         <v>15.99</v>
@@ -11845,7 +11758,7 @@
         <v>-55.746200000000002</v>
       </c>
       <c r="AF101" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="AG101">
         <v>0</v>

</xml_diff>

<commit_message>
final changes to dataset
</commit_message>
<xml_diff>
--- a/Fires.xlsx
+++ b/Fires.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Luis/Code/BigDataFinalProject/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60E2693-757C-B545-B306-1AC6284FB6BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38BE5F2-E2BD-3640-8FEA-4DEF9CFE064A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="68800" windowHeight="28300" xr2:uid="{D96FEB7F-44AB-FA47-9DDF-3B0615B72A44}"/>
   </bookViews>
@@ -1021,9 +1021,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C79AE7BB-29A4-0D4F-A0ED-DC6610B9D1DA}">
   <dimension ref="A1:AI101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>